<commit_message>
Update the main program and data
</commit_message>
<xml_diff>
--- a/sim/waypoints.xlsx
+++ b/sim/waypoints.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -16,8 +16,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,6 +54,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -343,36 +348,136 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>-37.713000000000001</v>
+      </c>
+      <c r="B1">
+        <v>-16.139700000000001</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>-26.090800000000002</v>
+      </c>
+      <c r="B2">
+        <v>-16.893899999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>-34.668799999999997</v>
+      </c>
+      <c r="B3">
+        <v>-28.9877</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>-16.049800000000001</v>
+      </c>
+      <c r="B4">
+        <v>-15.536300000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>-9.0131800000000002</v>
+      </c>
+      <c r="B5">
+        <v>-17.9497</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.5022</v>
+      </c>
+      <c r="B6">
+        <v>-15.687200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6.5622299999999996</v>
+      </c>
+      <c r="B7">
+        <v>-16.139700000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>-24.351400000000002</v>
+      </c>
+      <c r="B8">
+        <v>-28.357500000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>-15.180099999999999</v>
+      </c>
+      <c r="B9">
+        <v>-28.810099999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>-7.9062999999999999</v>
+      </c>
+      <c r="B10">
+        <v>-28.357500000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6.9575399999999998</v>
+      </c>
+      <c r="B11">
+        <v>-27.452500000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>8.9710599999999996</v>
+      </c>
+      <c r="B12">
+        <v>-32.300600000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>